<commit_message>
Began experimenting with dummy system to pull data from RTC into the Task Management System.
Total hours: 20.5
</commit_message>
<xml_diff>
--- a/Senior Project Tracking RTC.xlsx
+++ b/Senior Project Tracking RTC.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="2160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="2160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Investigation into how RTC works and how to pull from our version of it. Figured out basic commands for pulling from a stream.</t>
+  </si>
+  <si>
+    <t>Began experimenting with dummy system to pull data from RTC into the Task Management System.</t>
   </si>
 </sst>
 </file>
@@ -121,7 +124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -130,6 +133,7 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,14 +438,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L7"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -467,7 +472,7 @@
       </c>
       <c r="L1" s="7">
         <f>SUM(D:D)</f>
-        <v>12.5</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -481,7 +486,7 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D7" si="0">MOD(IF(ISBLANK(C2),B2, C2)-B2, 1)*24</f>
+        <f t="shared" ref="D2:D8" si="0">MOD(IF(ISBLANK(C2),B2, C2)-B2, 1)*24</f>
         <v>1.0000000000000004</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -585,6 +590,24 @@
       </c>
       <c r="E7" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>42412</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0.4375</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.77083333333333337</v>
+      </c>
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lots of updates. At 88.58 hours.
</commit_message>
<xml_diff>
--- a/Senior Project Tracking RTC.xlsx
+++ b/Senior Project Tracking RTC.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -72,6 +72,36 @@
   </si>
   <si>
     <t>Began experimenting with dummy system to pull data from RTC into the Task Management System.</t>
+  </si>
+  <si>
+    <t>Adding component to ensure that dependencies are loaded correctly for RTC.</t>
+  </si>
+  <si>
+    <t>Various RTC related things</t>
+  </si>
+  <si>
+    <t>Meeting for RTC update and path forward for what we want to do and how we want to do it.</t>
+  </si>
+  <si>
+    <t>Page Navigation</t>
+  </si>
+  <si>
+    <t>Finished Page Navigation</t>
+  </si>
+  <si>
+    <t>Working on presentation 1</t>
+  </si>
+  <si>
+    <t>Presenting</t>
+  </si>
+  <si>
+    <t>Working on stream pull functionality</t>
+  </si>
+  <si>
+    <t>Presenting initial demo of stream pull functionality</t>
+  </si>
+  <si>
+    <t>Touch-ups and troubleshooting.</t>
   </si>
 </sst>
 </file>
@@ -133,7 +163,7 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,20 +468,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
@@ -472,7 +500,7 @@
       </c>
       <c r="L1" s="7">
         <f>SUM(D:D)</f>
-        <v>20.5</v>
+        <v>88.583333333333329</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -486,7 +514,7 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D8" si="0">MOD(IF(ISBLANK(C2),B2, C2)-B2, 1)*24</f>
+        <f t="shared" ref="D2:D22" si="0">MOD(IF(ISBLANK(C2),B2, C2)-B2, 1)*24</f>
         <v>1.0000000000000004</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -593,7 +621,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8" s="6">
         <v>42412</v>
       </c>
       <c r="B8" s="2">
@@ -608,6 +636,258 @@
       </c>
       <c r="E8" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>42415</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>5.8333333333333321</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>42416</v>
+      </c>
+      <c r="B10" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>5.0000000000000009</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="6">
+        <v>42416</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000018</v>
+      </c>
+      <c r="E11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="6">
+        <v>42417</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="6">
+        <v>42418</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D13" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="6">
+        <v>42419</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D14" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>42422</v>
+      </c>
+      <c r="B15" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="C15" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>42422</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="C16" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="D16" s="3">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>42422</v>
+      </c>
+      <c r="B17" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="C17" s="2">
+        <v>0.6875</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" si="0"/>
+        <v>0.99999999999999911</v>
+      </c>
+      <c r="E17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>42423</v>
+      </c>
+      <c r="B18" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="C18" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" si="0"/>
+        <v>6.9999999999999991</v>
+      </c>
+      <c r="E18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>42424</v>
+      </c>
+      <c r="B19" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="C19" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>42425</v>
+      </c>
+      <c r="B20" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="C20" s="2">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="D20" s="3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>42426</v>
+      </c>
+      <c r="B21" s="2">
+        <v>0.28125</v>
+      </c>
+      <c r="C21" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D21" s="3">
+        <f t="shared" si="0"/>
+        <v>1.2499999999999996</v>
+      </c>
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="6">
+        <v>42426</v>
+      </c>
+      <c r="B22" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C22" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="D22" s="3">
+        <f t="shared" si="0"/>
+        <v>1.0000000000000004</v>
+      </c>
+      <c r="E22" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding recent updates to time tracking. Adding Presentation 2.pptx. At 102 hours.
</commit_message>
<xml_diff>
--- a/Senior Project Tracking RTC.xlsx
+++ b/Senior Project Tracking RTC.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -102,6 +102,18 @@
   </si>
   <si>
     <t>Touch-ups and troubleshooting.</t>
+  </si>
+  <si>
+    <t>Fixing bug preventing pull.</t>
+  </si>
+  <si>
+    <t>Looking into not duplicating workspaces every time we pull.</t>
+  </si>
+  <si>
+    <t>Trying to figure out how to push results back.</t>
+  </si>
+  <si>
+    <t>Preparing presentation 2.</t>
   </si>
 </sst>
 </file>
@@ -468,9 +480,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -500,7 +514,7 @@
       </c>
       <c r="L1" s="7">
         <f>SUM(D:D)</f>
-        <v>88.583333333333329</v>
+        <v>102.58333333333333</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -514,7 +528,7 @@
         <v>0.47916666666666669</v>
       </c>
       <c r="D2" s="3">
-        <f t="shared" ref="D2:D22" si="0">MOD(IF(ISBLANK(C2),B2, C2)-B2, 1)*24</f>
+        <f t="shared" ref="D2:D25" si="0">MOD(IF(ISBLANK(C2),B2, C2)-B2, 1)*24</f>
         <v>1.0000000000000004</v>
       </c>
       <c r="E2" s="1" t="s">
@@ -888,6 +902,78 @@
       </c>
       <c r="E22" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>42463</v>
+      </c>
+      <c r="B23" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="D23" s="3">
+        <f t="shared" si="0"/>
+        <v>1.9999999999999982</v>
+      </c>
+      <c r="E23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="6">
+        <v>42466</v>
+      </c>
+      <c r="B24" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="C24" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D24" s="3">
+        <f>MOD(IF(ISBLANK(C24),B24, C24)-B24, 1)*24</f>
+        <v>5.0000000000000009</v>
+      </c>
+      <c r="E24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="6">
+        <v>42467</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0.375</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="D25" s="3">
+        <f>MOD(IF(ISBLANK(C25),B25, C25)-B25, 1)*24</f>
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>42468</v>
+      </c>
+      <c r="B26" s="2">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="C26" s="2">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D26" s="3">
+        <f>MOD(IF(ISBLANK(C26),B26, C26)-B26, 1)*24</f>
+        <v>4</v>
+      </c>
+      <c r="E26" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>